<commit_message>
WANC revised and ready for publication (indicator 3/5)
</commit_message>
<xml_diff>
--- a/indicators/NO_WANC_001_002/metadata.xlsx
+++ b/indicators/NO_WANC_001_002/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanno.sandvik\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\61308-01_fu_intern_hanno_sandvik\ecRxiv_vann\indicators\NO_WANC_001_002\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2747C325-6E0E-4580-A6C9-A12F5657F766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25E7E73-0AC9-4445-842C-F9561A162596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5774BAF6-AFFD-43CB-8AE5-DFBA2C21B702}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{5774BAF6-AFFD-43CB-8AE5-DFBA2C21B702}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -692,12 +692,6 @@
     <t>Sandvik, H.</t>
   </si>
   <si>
-    <t>001.000</t>
-  </si>
-  <si>
-    <t>First complete version</t>
-  </si>
-  <si>
     <t>Scale - Transform - Aggregate (size-weighted arithmetic mean) - Truncate</t>
   </si>
   <si>
@@ -711,6 +705,12 @@
   </si>
   <si>
     <t>Acid-neutralising capacity (ANC)</t>
+  </si>
+  <si>
+    <t>002.000</t>
+  </si>
+  <si>
+    <t>Updated with 2024 data</t>
   </si>
 </sst>
 </file>
@@ -1172,7 +1172,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1202,7 +1202,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>197</v>
@@ -1216,7 +1216,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>197</v>
@@ -1230,7 +1230,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>199</v>
@@ -1385,7 +1385,7 @@
         <v>166</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>178</v>
@@ -1399,7 +1399,7 @@
         <v>167</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>168</v>
@@ -1425,7 +1425,7 @@
         <v>183</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>187</v>
@@ -1453,7 +1453,7 @@
         <v>194</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>196</v>

</xml_diff>

<commit_message>
new rendered version of five indicators (preliminarily adjusted to new vannmiljo API)
</commit_message>
<xml_diff>
--- a/indicators/NO_WANC_001_002/metadata.xlsx
+++ b/indicators/NO_WANC_001_002/metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\61308-01_fu_intern_hanno_sandvik\ecRxiv_vann\indicators\NO_WANC_001_002\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25E7E73-0AC9-4445-842C-F9561A162596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F29E6BA-8CC0-4F26-906F-7655E207C23B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{5774BAF6-AFFD-43CB-8AE5-DFBA2C21B702}"/>
   </bookViews>
@@ -707,10 +707,10 @@
     <t>Acid-neutralising capacity (ANC)</t>
   </si>
   <si>
-    <t>002.000</t>
-  </si>
-  <si>
-    <t>Updated with 2024 data</t>
+    <t>First complete version</t>
+  </si>
+  <si>
+    <t>001.000</t>
   </si>
 </sst>
 </file>
@@ -1385,7 +1385,7 @@
         <v>166</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>178</v>
@@ -1399,7 +1399,7 @@
         <v>167</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>168</v>

</xml_diff>